<commit_message>
sample num 6 is cleaned up
</commit_message>
<xml_diff>
--- a/Test-Data/Example6.xlsx
+++ b/Test-Data/Example6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI-MRO\Data\Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A825ABD-C50A-4125-ADEB-D7A95654E1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36720AD9-D003-457F-B643-06CCC83B8AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="3520" yWindow="5120" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
@@ -844,20 +844,20 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="3"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -880,7 +880,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -905,7 +905,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>102</v>
@@ -931,7 +931,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>103</v>
@@ -946,18 +946,17 @@
         <v>45748</v>
       </c>
       <c r="E4" s="9">
-        <f>C4+0.9</f>
-        <v>1.2611111111111111</v>
+        <v>0.26111111111111113</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -972,8 +971,7 @@
         <v>45748</v>
       </c>
       <c r="E5" s="9">
-        <f>C5+0.82</f>
-        <v>1.2088888888888889</v>
+        <v>0.2088888888888889</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
@@ -983,7 +981,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -998,18 +996,17 @@
         <v>45748</v>
       </c>
       <c r="E6" s="9">
-        <f>C6+0.543</f>
-        <v>1.0117500000000001</v>
+        <v>1.1342592592592592E-2</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>0.54300000000000015</v>
+        <v>0.54259259259259252</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1034,7 +1031,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1059,7 +1056,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1074,18 +1071,17 @@
         <v>45748</v>
       </c>
       <c r="E9" s="9">
-        <f>C9+0.61</f>
-        <v>1.1724999999999999</v>
+        <v>0.17249999999999999</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="0"/>
-        <v>0.60999999999999988</v>
+        <v>0.61</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1100,8 +1096,7 @@
         <v>45748</v>
       </c>
       <c r="E10" s="9">
-        <f>C10+0.51</f>
-        <v>1.1176388888888888</v>
+        <v>0.11763888888888889</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="0"/>
@@ -1111,7 +1106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1126,18 +1121,17 @@
         <v>45749</v>
       </c>
       <c r="E11" s="9">
-        <f>C11+0.753</f>
-        <v>1.4509166666666666</v>
+        <v>0.45091435185185186</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>0.753</v>
+        <v>0.75299768518518517</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1152,18 +1146,17 @@
         <v>45749</v>
       </c>
       <c r="E12" s="9">
-        <f>C12+0.673</f>
-        <v>1.3986944444444445</v>
+        <v>0.39869212962962958</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
-        <v>0.67300000000000004</v>
+        <v>0.6729976851851851</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1178,18 +1171,17 @@
         <v>45749</v>
       </c>
       <c r="E13" s="9">
-        <f>C13+0.784</f>
-        <v>1.5617777777777779</v>
+        <v>0.56177083333333333</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>0.78400000000000014</v>
+        <v>0.78399305555555554</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1204,18 +1196,17 @@
         <v>45749</v>
       </c>
       <c r="E14" s="9">
-        <f>C14+0.92</f>
-        <v>1.7220833333333334</v>
+        <v>0.7220833333333333</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>0.91999999999999993</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1230,18 +1221,17 @@
         <v>45749</v>
       </c>
       <c r="E15" s="9">
-        <f>C15+0.78</f>
-        <v>1.5890277777777779</v>
+        <v>0.58902777777777782</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="0"/>
-        <v>0.78000000000000014</v>
+        <v>0.78</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1256,8 +1246,7 @@
         <v>45749</v>
       </c>
       <c r="E16" s="9">
-        <f>C16+0.86</f>
-        <v>1.6759722222222222</v>
+        <v>0.6759722222222222</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="0"/>
@@ -1267,7 +1256,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1282,8 +1271,7 @@
         <v>45749</v>
       </c>
       <c r="E17" s="9">
-        <f>C17+0.79</f>
-        <v>1.6476388888888889</v>
+        <v>0.64763888888888888</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" si="0"/>
@@ -1293,7 +1281,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1308,18 +1296,17 @@
         <v>45749</v>
       </c>
       <c r="E18" s="9">
-        <f>C18+0.9</f>
-        <v>1.7854166666666667</v>
+        <v>0.78541666666666676</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.90000000000000013</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1344,7 +1331,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1369,7 +1356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1394,131 +1381,131 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B53" s="8"/>
       <c r="D53" s="8"/>
     </row>
@@ -1535,18 +1522,18 @@
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="3"/>
-    <col min="4" max="4" width="10.875" style="4"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1563,7 +1550,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1587,7 +1574,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1611,7 +1598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1622,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1646,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1683,7 +1670,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1694,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1731,7 +1718,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1755,7 +1742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1779,7 +1766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1803,7 +1790,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1827,7 +1814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1851,7 +1838,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1875,7 +1862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1899,7 +1886,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1923,7 +1910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1947,7 +1934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1971,7 +1958,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1995,7 +1982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2020,7 +2007,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2045,7 +2032,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2070,7 +2057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2095,7 +2082,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2120,7 +2107,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2145,7 +2132,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -2162,13 +2149,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>109</v>
       </c>
@@ -2176,7 +2163,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2187,7 +2174,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2198,7 +2185,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2209,7 +2196,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2220,7 +2207,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2231,7 +2218,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2242,7 +2229,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2253,7 +2240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2264,7 +2251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2275,7 +2262,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2286,7 +2273,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2297,7 +2284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2308,7 +2295,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2319,7 +2306,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2330,7 +2317,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2341,7 +2328,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2352,7 +2339,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2363,7 +2350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2374,7 +2361,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2385,7 +2372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2396,7 +2383,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2407,7 +2394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2418,7 +2405,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2429,7 +2416,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2440,7 +2427,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2451,7 +2438,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2462,7 +2449,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2473,7 +2460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2484,7 +2471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2495,7 +2482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2506,7 +2493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2517,7 +2504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2528,7 +2515,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2539,7 +2526,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2550,7 +2537,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2561,7 +2548,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
typo removed from the excel sheet
</commit_message>
<xml_diff>
--- a/Test-Data/Example6.xlsx
+++ b/Test-Data/Example6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36720AD9-D003-457F-B643-06CCC83B8AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA5D2D-859C-4307-A169-26FB9AF0071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="5120" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="110" yWindow="2850" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
@@ -382,9 +382,6 @@
     <t>WP8, WP11, WP18</t>
   </si>
   <si>
-    <t>WP11, W22</t>
-  </si>
-  <si>
     <t>WP5, WP8</t>
   </si>
   <si>
@@ -419,6 +416,9 @@
   </si>
   <si>
     <t>WP6, WP14, WP22</t>
+  </si>
+  <si>
+    <t>WP11, WP22</t>
   </si>
 </sst>
 </file>
@@ -844,7 +844,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -978,7 +978,7 @@
         <v>0.82000000000000006</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -1003,7 +1003,7 @@
         <v>0.54259259259259252</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -1028,7 +1028,7 @@
         <v>0.39930555555555558</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -1053,7 +1053,7 @@
         <v>0.46527777777777768</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -1078,7 +1078,7 @@
         <v>0.61</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -1153,7 +1153,7 @@
         <v>0.6729976851851851</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -1203,7 +1203,7 @@
         <v>0.91999999999999993</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -1228,7 +1228,7 @@
         <v>0.78</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -1253,7 +1253,7 @@
         <v>0.86</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -1278,7 +1278,7 @@
         <v>0.79</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -1303,7 +1303,7 @@
         <v>0.90000000000000013</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -1328,7 +1328,7 @@
         <v>0.33333333333333337</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
@@ -1378,7 +1378,7 @@
         <v>0.31597222222222221</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>

</xml_diff>